<commit_message>
Import template: remove Payment Frequency from Payouts sheet (redundant; present on Models)
</commit_message>
<xml_diff>
--- a/app/static/import_templates/payroll_import_template.xlsx
+++ b/app/static/import_templates/payroll_import_template.xlsx
@@ -520,7 +520,6 @@
       <c r="H2" t="n">
         <v>4500</v>
       </c>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -578,7 +577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,11 +613,6 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Payment Frequency</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>Notes</t>
         </is>
       </c>
@@ -649,11 +643,6 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Monthly</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>June retainer</t>
         </is>
       </c>
@@ -684,11 +673,6 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Biweekly</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t>Campaign launch</t>
         </is>
       </c>
@@ -718,11 +702,6 @@
         </is>
       </c>
       <c r="F4" t="inlineStr">
-        <is>
-          <t>Biweekly</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
         <is>
           <t>Adjusted schedule</t>
         </is>

</xml_diff>

<commit_message>
feat(template): add dropdowns to import template (Models payment_frequency; Payouts status) including all allowed types; add maintenance script to update validations
</commit_message>
<xml_diff>
--- a/app/static/import_templates/payroll_import_template.xlsx
+++ b/app/static/import_templates/payroll_import_template.xlsx
@@ -567,6 +567,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="G2:G1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"weekly,biweekly,monthly"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -708,6 +713,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="D2:D1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"paid,on_hold,not_paid"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Import template: add weekly sample row (Models) and on_hold sample row (Payouts); include idempotent script to maintain samples
</commit_message>
<xml_diff>
--- a/app/static/import_templates/payroll_import_template.xlsx
+++ b/app/static/import_templates/payroll_import_template.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,6 +564,46 @@
         <is>
           <t>0xABCDEF1234567890</t>
         </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>M-003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sample Weekly Model</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>WeeklySample</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>weekly</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -712,6 +752,31 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>M-003</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>on_hold</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">

</xml_diff>

<commit_message>
Import template: add Adhoc sheet with status dropdown and example row; extend validation and sample scripts to manage Adhoc
</commit_message>
<xml_diff>
--- a/app/static/import_templates/payroll_import_template.xlsx
+++ b/app/static/import_templates/payroll_import_template.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Models" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Payouts" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Adhoc" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -607,7 +608,10 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="G2:G1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"weekly,biweekly,monthly"</formula1>
+    </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"weekly,biweekly,monthly"</formula1>
     </dataValidation>
@@ -778,11 +782,100 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="D2:D1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"paid,on_hold,not_paid"</formula1>
+    </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"paid,on_hold,not_paid"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pay_date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>M-003</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-11-05</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Bonus</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Sample adhoc payment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="D2:D1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"pending,paid,cancelled"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Template: add second Adhoc sample row with status=paid; update samples script to ensure both pending and paid examples
</commit_message>
<xml_diff>
--- a/app/static/import_templates/payroll_import_template.xlsx
+++ b/app/static/import_templates/payroll_import_template.xlsx
@@ -800,7 +800,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,6 +870,36 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>M-004</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-11-05</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>75</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>paid</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Reimbursement</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Sample paid adhoc payment</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">

</xml_diff>